<commit_message>
Integrated uncommitted changes sitting on yilgarn server
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSrunSTDS.xlsx
+++ b/Test-Data/WiscSIMSrunSTDS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1BF806-2492-6F49-A100-AD9F015696ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8FBB7B-DE2D-2C4E-BC58-ADEFB5C99C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="16220" xr2:uid="{4BB3FC3E-1443-2C4F-A4D1-E3012F903B60}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>StdName</t>
   </si>
@@ -56,9 +56,21 @@
     <t>REGEX</t>
   </si>
   <si>
+    <t>UWC.*3</t>
+  </si>
+  <si>
+    <t>UWQ.*1</t>
+  </si>
+  <si>
+    <t>UW.*Arg.*7</t>
+  </si>
+  <si>
     <t>UW6220</t>
   </si>
   <si>
+    <t>UW.*6220</t>
+  </si>
+  <si>
     <t>UW6250</t>
   </si>
   <si>
@@ -101,70 +113,46 @@
     <t>UWAnk5opq</t>
   </si>
   <si>
-    <t>StdType</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>Calib</t>
-  </si>
-  <si>
-    <t>RunCalib</t>
-  </si>
-  <si>
-    <t>UWC\\D*3</t>
-  </si>
-  <si>
-    <t>UWQ\\D*1</t>
-  </si>
-  <si>
-    <t>UW.*Arg\\D*7</t>
-  </si>
-  <si>
-    <t>UW\\D*6220</t>
-  </si>
-  <si>
-    <t>UW\\D*6250</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*10</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*11</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*7</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*8</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*4</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*9</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*1</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*2</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*3</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*12</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*5.*opq</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*6.*a</t>
-  </si>
-  <si>
-    <t>UW.*Ank\\D*5.*cl</t>
+    <t>UW.*6250</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*10</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*11</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*7</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*8</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*4</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*9</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*1</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*2</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*3</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*5.*cl</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*6.*a</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*12</t>
+  </si>
+  <si>
+    <t>UW.*Ank.*5.*opq</t>
   </si>
 </sst>
 </file>
@@ -516,21 +504,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055469BC-4AEE-DB42-A546-EDD0413F37E8}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,11 +531,8 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -558,13 +543,10 @@
         <v>12.49</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -572,13 +554,10 @@
         <v>12.33</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -589,15 +568,12 @@
         <v>-10.84</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0.84</v>
@@ -606,15 +582,12 @@
         <v>22.6</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1.29</v>
@@ -623,15 +596,12 @@
         <v>21.4</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>-1.52</v>
@@ -640,29 +610,23 @@
         <v>19.55</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>10.49</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>-8.36</v>
@@ -671,15 +635,12 @@
         <v>11.38</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>-4.1500000000000004</v>
@@ -688,29 +649,23 @@
         <v>9.19</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>9.2200000000000006</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>-6.99</v>
@@ -719,15 +674,12 @@
         <v>11.68</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>-7.38</v>
@@ -736,15 +688,12 @@
         <v>15.87</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>-7.35</v>
@@ -753,15 +702,12 @@
         <v>15.9</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>-7.34</v>
@@ -770,15 +716,12 @@
         <v>15.82</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>-4.57</v>
@@ -787,15 +730,12 @@
         <v>17.11</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>-4.4000000000000004</v>
@@ -804,38 +744,29 @@
         <v>15.99</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
       </c>
       <c r="B18">
         <v>3.19</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>-4.59</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Material designation for this table
Allow for running standards to allow for material designation.
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSrunSTDS.xlsx
+++ b/Test-Data/WiscSIMSrunSTDS.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C662B600-0B04-A549-9679-2DED825C16D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF21CD5-BD33-084E-BBC3-F2F7C21B4400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="16220" xr2:uid="{4BB3FC3E-1443-2C4F-A4D1-E3012F903B60}"/>
+    <workbookView xWindow="780" yWindow="640" windowWidth="27640" windowHeight="16220" xr2:uid="{4BB3FC3E-1443-2C4F-A4D1-E3012F903B60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>StdName</t>
   </si>
@@ -171,6 +171,42 @@
   </si>
   <si>
     <t>UWG\D*2</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Carbonate</t>
+  </si>
+  <si>
+    <t>Quartz</t>
+  </si>
+  <si>
+    <t>Aragonite</t>
+  </si>
+  <si>
+    <t>Dolomite</t>
+  </si>
+  <si>
+    <t>Garnet</t>
+  </si>
+  <si>
+    <t>UWZ-1</t>
+  </si>
+  <si>
+    <t>KIM-5</t>
+  </si>
+  <si>
+    <t>KIM\D*5</t>
+  </si>
+  <si>
+    <t>Zircon</t>
+  </si>
+  <si>
+    <t>UWZ\D*1</t>
+  </si>
+  <si>
+    <t>Ankerite</t>
   </si>
 </sst>
 </file>
@@ -523,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055469BC-4AEE-DB42-A546-EDD0413F37E8}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +573,7 @@
     <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,8 +589,11 @@
       <c r="E1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -570,8 +609,11 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -584,8 +626,11 @@
       <c r="E3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -601,8 +646,11 @@
       <c r="E4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -618,8 +666,11 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -635,8 +686,11 @@
       <c r="E6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -652,8 +706,11 @@
       <c r="E7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -666,8 +723,11 @@
       <c r="E8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -683,8 +743,11 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -700,8 +763,11 @@
       <c r="E10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -714,8 +780,11 @@
       <c r="E11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -731,8 +800,11 @@
       <c r="E12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -748,8 +820,11 @@
       <c r="E13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -765,8 +840,11 @@
       <c r="E14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -782,8 +860,11 @@
       <c r="E15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -799,8 +880,11 @@
       <c r="E16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -816,8 +900,11 @@
       <c r="E17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -830,8 +917,11 @@
       <c r="E18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -844,8 +934,11 @@
       <c r="E19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -857,6 +950,40 @@
       </c>
       <c r="E20" t="s">
         <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <v>5.09</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more standard regex keys
</commit_message>
<xml_diff>
--- a/Test-Data/WiscSIMSrunSTDS.xlsx
+++ b/Test-Data/WiscSIMSrunSTDS.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macrostrat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF21CD5-BD33-084E-BBC3-F2F7C21B4400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3CE73F-5CAA-824D-992F-580596434611}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="640" windowWidth="27640" windowHeight="16220" xr2:uid="{4BB3FC3E-1443-2C4F-A4D1-E3012F903B60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>StdName</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>Ankerite</t>
+  </si>
+  <si>
+    <t>UWC-1</t>
+  </si>
+  <si>
+    <t>UWC\D*1</t>
+  </si>
+  <si>
+    <t>UWW-1</t>
+  </si>
+  <si>
+    <t>UWW\D*1</t>
+  </si>
+  <si>
+    <t>Something</t>
   </si>
 </sst>
 </file>
@@ -559,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055469BC-4AEE-DB42-A546-EDD0413F37E8}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,6 +1001,34 @@
         <v>55</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>